<commit_message>
Reformat code & add some missing 'Step' info
</commit_message>
<xml_diff>
--- a/target/classes/Credentials.xlsx
+++ b/target/classes/Credentials.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>privacyType</t>
   </si>
@@ -49,12 +49,16 @@
   </si>
   <si>
     <t>Kuku 2</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -390,23 +394,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.44140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.6640625"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="16.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>6</v>
       </c>
     </row>
@@ -420,6 +424,9 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
@@ -430,6 +437,9 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>